<commit_message>
Alterações de ortografia + restrição de arquivo
</commit_message>
<xml_diff>
--- a/undefined.xlsx
+++ b/undefined.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -20,13 +20,8 @@
       <sz val="12"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <color rgb="FFB51F1F"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none">
         <bgColor/>
@@ -34,12 +29,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125">
-        <bgColor/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCC3B3"/>
         <bgColor/>
       </patternFill>
     </fill>
@@ -63,11 +52,10 @@
   <cellStyleXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,38 +690,20 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="str">
+      <c r="A27" s="2" t="str">
         <v>26/07/2019  Fri</v>
       </c>
       <c r="B27" s="2" t="str">
         <v>(N)</v>
       </c>
-      <c r="C27" s="3" t="str">
-        <v/>
-      </c>
-      <c r="D27" s="3" t="str">
-        <v/>
-      </c>
-      <c r="E27" s="3" t="str">
-        <v/>
-      </c>
-      <c r="F27" s="3" t="str">
-        <v/>
-      </c>
-      <c r="G27" s="3" t="str">
-        <v/>
-      </c>
-      <c r="H27" s="3" t="str">
-        <v/>
-      </c>
-      <c r="I27" s="3" t="str">
-        <v/>
-      </c>
-      <c r="J27" s="3" t="str">
-        <v/>
-      </c>
-      <c r="K27" s="3" t="str">
-        <v>Débito Banco Horas</v>
+      <c r="C27" s="2" t="str">
+        <v>07:47</v>
+      </c>
+      <c r="D27" s="2" t="str">
+        <v>11:46</v>
+      </c>
+      <c r="F27" s="2" t="str">
+        <v>16:54</v>
       </c>
     </row>
     <row r="28">
@@ -1048,38 +1018,20 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="str">
+      <c r="A47" s="2" t="str">
         <v>15/08/2019  Thu</v>
       </c>
       <c r="B47" s="2" t="str">
         <v>(N)</v>
       </c>
-      <c r="C47" s="3" t="str">
-        <v/>
-      </c>
-      <c r="D47" s="3" t="str">
-        <v/>
-      </c>
-      <c r="E47" s="3" t="str">
-        <v/>
-      </c>
-      <c r="F47" s="3" t="str">
-        <v/>
-      </c>
-      <c r="G47" s="3" t="str">
-        <v/>
-      </c>
-      <c r="H47" s="3" t="str">
-        <v/>
-      </c>
-      <c r="I47" s="3" t="str">
-        <v/>
-      </c>
-      <c r="J47" s="3" t="str">
-        <v/>
-      </c>
-      <c r="K47" s="3" t="str">
-        <v>Débito Banco Horas</v>
+      <c r="C47" s="2" t="str">
+        <v>07:57</v>
+      </c>
+      <c r="D47" s="2" t="str">
+        <v>11:36</v>
+      </c>
+      <c r="F47" s="2" t="str">
+        <v>17:14</v>
       </c>
     </row>
     <row r="48">

</xml_diff>